<commit_message>
added new reports and mior UI changes
</commit_message>
<xml_diff>
--- a/assets/reports/09-20-2023to09-26-2023_feesReport.xlsx
+++ b/assets/reports/09-20-2023to09-26-2023_feesReport.xlsx
@@ -14,113 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35" count="35">
-  <x:si>
-    <x:t>AdmissionNo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Class</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Amount</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payment_Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Receipt_No</x:t>
-  </x:si>
-  <x:si>
-    <x:t>isCancelled</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SchoolCode</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PaidTo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>createdAt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>updatedAt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15253</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-09-24T16:11:24.509Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pay</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SVVN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>rohit@mail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fees</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Sep 24 2023 21:41:24 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Sep 24 2023 21:41:24 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15252</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-09-26T08:35:52.378Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>chf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:05:52 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:05:52 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-09-26T08:36:02.450Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ik</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:06:02 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:06:02 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15251</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-09-26T08:36:22.165Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mlkhl</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:06:22 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue Sep 26 2023 14:06:22 GMT+0530 (India Standard Time)</x:t>
-  </x:si>
-</x:sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,196 +375,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:12">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="J1" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="K1" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="L1" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:12">
-      <x:c r="A2" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="n">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:12">
-      <x:c r="A3" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="n">
-        <x:v>214</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="n">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="K3" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L3" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:12">
-      <x:c r="A4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="n">
-        <x:v>415</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="K4" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="L4" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:12">
-      <x:c r="A5" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="n">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="n">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="J5" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="K5" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="L5" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="1" spans="1:0"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>